<commit_message>
Remove outdated robot dataset preparation notebook and its checkpoint
</commit_message>
<xml_diff>
--- a/robot/data/lp1.xls( failure1).xlsx
+++ b/robot/data/lp1.xls( failure1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\merih\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\merih\Downloads\ml_project\robot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F33093-5712-4708-AFFC-E4DCD5564BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186D6B43-75FD-4546-897C-8C8B106F3F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="340" windowWidth="14400" windowHeight="7360" xr2:uid="{17CAAEB0-4035-4C2F-81D3-A762B764737C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{17CAAEB0-4035-4C2F-81D3-A762B764737C}"/>
   </bookViews>
   <sheets>
     <sheet name="lp1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="11">
   <si>
     <t>normal</t>
   </si>
@@ -45,24 +45,6 @@
   </si>
   <si>
     <t>fr_collision</t>
-  </si>
-  <si>
-    <t>FX</t>
-  </si>
-  <si>
-    <t>FY</t>
-  </si>
-  <si>
-    <t>FZ</t>
-  </si>
-  <si>
-    <t>TX</t>
-  </si>
-  <si>
-    <t>TY</t>
-  </si>
-  <si>
-    <t>TZ</t>
   </si>
   <si>
     <t>Fx</t>
@@ -946,33 +928,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A905687-697E-4BE0-97FE-5CB5CD0AAC6B}">
   <dimension ref="A1:G1583"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="A658" workbookViewId="0">
+      <selection activeCell="B668" sqref="B668"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -12263,24 +12245,6 @@
     <row r="668" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A668" t="s">
         <v>2</v>
-      </c>
-      <c r="B668" t="s">
-        <v>4</v>
-      </c>
-      <c r="C668" t="s">
-        <v>5</v>
-      </c>
-      <c r="D668" t="s">
-        <v>6</v>
-      </c>
-      <c r="E668" t="s">
-        <v>7</v>
-      </c>
-      <c r="F668" t="s">
-        <v>8</v>
-      </c>
-      <c r="G668" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="669" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>